<commit_message>
added GCP pricing, overview of GPU options
</commit_message>
<xml_diff>
--- a/sagemaker pricing.xlsx
+++ b/sagemaker pricing.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairjones/Desktop/descriptiveworld/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3565CB-8AA5-A947-AC5A-2152092F471D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAAB99A-C854-1041-8082-A3C1EBE6DD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15920" xr2:uid="{CE9B920F-D75E-2E44-AE3B-DFBDD13E397D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15860" activeTab="1" xr2:uid="{CE9B920F-D75E-2E44-AE3B-DFBDD13E397D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GPU Options" sheetId="4" r:id="rId1"/>
+    <sheet name="AWS" sheetId="1" r:id="rId2"/>
+    <sheet name="Notebook Cost Estimate" sheetId="3" r:id="rId3"/>
+    <sheet name="GCP" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>ml.p3.2xlarge</t>
   </si>
@@ -42,9 +45,6 @@
     <t>$ per notebook per 24 hours</t>
   </si>
   <si>
-    <t>Compute Type: Accelerated Computing Instances</t>
-  </si>
-  <si>
     <t>V CPU: 8</t>
   </si>
   <si>
@@ -57,9 +57,6 @@
     <t>GPU: 1</t>
   </si>
   <si>
-    <t>Network Performance: N/A</t>
-  </si>
-  <si>
     <t>Storage: EBS only</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>GPU Memory: 0</t>
   </si>
   <si>
-    <t>Compute Type: Standard Instances</t>
-  </si>
-  <si>
     <t>V CPU: 2</t>
   </si>
   <si>
@@ -180,13 +174,74 @@
     <t>batch size</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>exp2</t>
-  </si>
-  <si>
-    <t>End</t>
+    <t>NVIDIA Tesla K80</t>
+  </si>
+  <si>
+    <t>GPU Memory: 12 GB</t>
+  </si>
+  <si>
+    <t>GPU: 2</t>
+  </si>
+  <si>
+    <t>GPU Memory: 24 GB</t>
+  </si>
+  <si>
+    <t>NVIDIA Tesla V100</t>
+  </si>
+  <si>
+    <t>GPU Memory: 16 GB</t>
+  </si>
+  <si>
+    <t>GPU Memory: 32 GB</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/choosing-the-right-gpu-for-deep-learning-on-aws-d69c157d8c86</t>
+  </si>
+  <si>
+    <t>NVIDIA Tesla T4</t>
+  </si>
+  <si>
+    <t>similar to AWS G4DN</t>
+  </si>
+  <si>
+    <t>similar to AWS P2</t>
+  </si>
+  <si>
+    <t>similar to AWS P3</t>
+  </si>
+  <si>
+    <t>Newer than K80</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GPU Memory: 16 GB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t>(by examining nvidia-smi on running notebook)</t>
+    </r>
+  </si>
+  <si>
+    <t>ml.p2.xlarge</t>
+  </si>
+  <si>
+    <t>GPU Memory: 12 GB?</t>
+  </si>
+  <si>
+    <t>Tesla T4</t>
+  </si>
+  <si>
+    <t>Tesla V100</t>
+  </si>
+  <si>
+    <t>K80</t>
+  </si>
+  <si>
+    <t>GPU Generation</t>
   </si>
 </sst>
 </file>
@@ -196,9 +251,9 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,8 +313,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +366,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -317,7 +393,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -342,11 +418,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -364,6 +444,116 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>802114</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5706C2A7-C29B-474E-BA99-1C673A43A249}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825500" y="812800"/>
+          <a:ext cx="9882614" cy="2527300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE487D3-7EFD-814C-88DB-CC6B47715E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="812800" y="3835400"/>
+          <a:ext cx="12700000" cy="9169400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -662,14 +852,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1784305-01BD-6244-84E5-2E47CDF6F41A}">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AEDBB6-F4A0-F346-86D8-94B36B32FD72}">
-  <dimension ref="B2:L56"/>
+  <dimension ref="B2:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -682,9 +893,9 @@
     <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="34">
+    <row r="2" spans="2:7" ht="34">
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="16" t="s">
@@ -692,425 +903,713 @@
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+        <v>18</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="2:6" ht="21">
+    <row r="4" spans="2:7" ht="21">
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5">
         <v>2.4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="F8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="F9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="F10" s="2" t="s">
+    <row r="8" spans="2:7">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="2:7" ht="21">
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5.52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="F12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" ht="21">
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="2:6" ht="21">
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="5">
-        <v>5.52</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="D14" s="5">
+        <v>17.670000000000002</v>
+      </c>
       <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="F16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
-      <c r="F15" s="3" t="s">
+    <row r="17" spans="2:11">
+      <c r="F17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="F18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
-      <c r="F16" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
-      <c r="F17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
-      <c r="F18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="20">
-        <v>0.48958333333333331</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:11">
       <c r="F19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
-      <c r="F20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:12" ht="21">
-      <c r="B22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="5">
-        <v>17.670000000000002</v>
-      </c>
-      <c r="F22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="2:11" ht="21">
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="5">
+        <f>24*0.9</f>
+        <v>21.6</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="F22" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="F24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="F25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="F26" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="2:11" ht="21">
+      <c r="B28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>91.8</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:12">
-      <c r="F23" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12">
-      <c r="F24" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12">
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12">
-      <c r="F26" s="3" t="s">
+      <c r="G28" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="F29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="17"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="F31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="17"/>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K26" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12">
-      <c r="F27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" t="s">
-        <v>44</v>
-      </c>
-      <c r="K27" s="22">
-        <v>52000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12">
-      <c r="F28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="22">
-        <f>L28*K27</f>
-        <v>41600</v>
-      </c>
-      <c r="L28" s="19">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12">
-      <c r="F29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K29" s="22">
-        <f>K27-K28</f>
-        <v>10400</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="J30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K30">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="21">
-      <c r="B31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="5">
-        <v>91.8</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12">
-      <c r="F32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32">
-        <v>300</v>
-      </c>
+      <c r="K32" s="17"/>
     </row>
     <row r="33" spans="2:11">
       <c r="F33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J33" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="22">
-        <f>K31*K32</f>
-        <v>4800</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="K33" s="17"/>
     </row>
     <row r="34" spans="2:11">
-      <c r="F34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>41</v>
-      </c>
-      <c r="K34">
-        <f>K33/60</f>
-        <v>80</v>
-      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:11">
-      <c r="F35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J35" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" s="18">
-        <f>K34/24</f>
-        <v>3.3333333333333335</v>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="8">
+        <v>117.36</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="2:11">
-      <c r="F36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36">
-        <f>ROUNDUP(K35,0)</f>
-        <v>4</v>
+      <c r="F36" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="2:11">
       <c r="F37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K37" s="17">
-        <f>D31</f>
-        <v>91.8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="2:11">
-      <c r="F38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" t="s">
-        <v>36</v>
-      </c>
-      <c r="K38" s="17">
-        <f>K36*K37</f>
-        <v>367.2</v>
+      <c r="F38" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="F39" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="8">
-        <v>117.36</v>
-      </c>
       <c r="F40" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="F41" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" spans="2:11">
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="8">
+        <v>352.51</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="43" spans="2:11">
-      <c r="F43" s="2" t="s">
-        <v>13</v>
+      <c r="F43" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="F44" s="1" t="s">
-        <v>28</v>
+      <c r="F44" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:11">
-      <c r="F45" s="2" t="s">
-        <v>7</v>
+      <c r="F45" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="F46" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:11">
       <c r="F47" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11">
-      <c r="B48" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD07A0C7-2929-A841-84EB-213D82DF3C14}">
+  <dimension ref="B3:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="C3" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="21">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="21">
+        <f>D5*C4</f>
+        <v>41600</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="21">
+        <f>C4-C5</f>
+        <v>10400</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" t="s">
+      <c r="C8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="21">
+        <f>C8*C9</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <f>C10/60</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="18">
+        <f>C11/24</f>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <f>ROUNDUP(C12,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="17">
+        <f>AWS!D21</f>
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="8">
-        <v>352.51</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="F50" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="F51" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="F52" s="2" t="s">
+      <c r="C15" s="17">
+        <f>C13*C14</f>
+        <v>86.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EDB817-2E12-174F-83CB-9E9E73257F1E}">
+  <dimension ref="B2:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="6" max="6" width="55.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="34">
+      <c r="B2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="2:9" ht="21">
+      <c r="B4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5">
+        <f>0.386*24</f>
+        <v>9.2639999999999993</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="F5" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="F6" s="22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
-      <c r="F53" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="F54" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="F55" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6">
-      <c r="F56" s="2" t="s">
-        <v>32</v>
+    <row r="7" spans="2:9">
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="2:9" ht="21">
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="5">
+        <f>0.631*24</f>
+        <v>15.144</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="F10" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="F11" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="2:9" ht="21">
+      <c r="B14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="5">
+        <f>0.456*24</f>
+        <v>10.944000000000001</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="F15" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="F16" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="F17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
+    </row>
+    <row r="19" spans="2:7" ht="21">
+      <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="5">
+        <f>0.771*24</f>
+        <v>18.504000000000001</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="F20" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="F21" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="F22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="2:7" ht="21">
+      <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="5">
+        <f>1.877*24</f>
+        <v>45.048000000000002</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="F25" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="F26" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="F27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="2:7" ht="21">
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5">
+        <f>3.613*24</f>
+        <v>86.712000000000003</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="F30" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="F31" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="F32" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>